<commit_message>
[FIX] Correção de erro ao editar o produto
</commit_message>
<xml_diff>
--- a/Artefatos/planejamento-sprints.xlsx
+++ b/Artefatos/planejamento-sprints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25803"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9D68FA6-9B1D-4197-9725-58C772E7A22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7264F9A9-90EE-4780-A773-B7639612831E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do Projeto" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -378,7 +379,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="120">
   <si>
     <t>PONTIFÍCIA UNIVERSIDADE CATÓLICA DE MINAS GERAIS</t>
   </si>
@@ -603,9 +604,6 @@
     <t>Cliente visualiza detalhes do produto</t>
   </si>
   <si>
-    <t>Tarefas Criadas</t>
-  </si>
-  <si>
     <t>Cliente realiza avaliação</t>
   </si>
   <si>
@@ -622,6 +620,9 @@
   </si>
   <si>
     <t>Usuário realiza cadastro</t>
+  </si>
+  <si>
+    <t>Tarefas Criadas</t>
   </si>
   <si>
     <t>Usuário realiza login</t>
@@ -745,6 +746,27 @@
   </si>
   <si>
     <t>SPRINT #4</t>
+  </si>
+  <si>
+    <t>Nikolas Louret</t>
+  </si>
+  <si>
+    <t>Gabriel Souza</t>
+  </si>
+  <si>
+    <t>Produção da identidade visual</t>
+  </si>
+  <si>
+    <t>Interface de Usuário</t>
+  </si>
+  <si>
+    <t>Casos de uso</t>
+  </si>
+  <si>
+    <t>Diagarama de classes</t>
+  </si>
+  <si>
+    <t>Planejamento da Sprint 5</t>
   </si>
   <si>
     <t>SPRINT #5</t>
@@ -3530,7 +3552,7 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3970,7 +3992,7 @@
   </sheetPr>
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
+    <sheetView topLeftCell="B13" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:E13"/>
     </sheetView>
   </sheetViews>
@@ -4341,7 +4363,7 @@
       </c>
       <c r="I102" s="55">
         <f>'Sprint #3'!I$61</f>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="J102" s="53"/>
       <c r="K102" s="54" t="str">
@@ -5468,8 +5490,8 @@
   </sheetPr>
   <dimension ref="A1:R1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5918,7 +5940,7 @@
       <c r="F31" s="93"/>
       <c r="G31" s="94"/>
       <c r="H31" s="12" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1">
@@ -5948,7 +5970,7 @@
       <c r="F33" s="93"/>
       <c r="G33" s="94"/>
       <c r="H33" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15.75" customHeight="1">
@@ -5956,14 +5978,14 @@
         <v>13</v>
       </c>
       <c r="C34" s="83" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="93"/>
       <c r="E34" s="93"/>
       <c r="F34" s="93"/>
       <c r="G34" s="94"/>
       <c r="H34" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="18" customHeight="1">
@@ -5971,14 +5993,14 @@
         <v>14</v>
       </c>
       <c r="C35" s="83" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="93"/>
       <c r="E35" s="93"/>
       <c r="F35" s="93"/>
       <c r="G35" s="94"/>
       <c r="H35" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="18" customHeight="1">
@@ -5986,14 +6008,14 @@
         <v>15</v>
       </c>
       <c r="C36" s="83" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="93"/>
       <c r="E36" s="93"/>
       <c r="F36" s="93"/>
       <c r="G36" s="94"/>
       <c r="H36" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="18" customHeight="1">
@@ -6001,14 +6023,14 @@
         <v>16</v>
       </c>
       <c r="C37" s="83" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" s="93"/>
       <c r="E37" s="93"/>
       <c r="F37" s="93"/>
       <c r="G37" s="94"/>
       <c r="H37" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="18" customHeight="1">
@@ -6016,7 +6038,7 @@
         <v>17</v>
       </c>
       <c r="C38" s="83" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" s="93"/>
       <c r="E38" s="93"/>
@@ -6031,14 +6053,14 @@
         <v>18</v>
       </c>
       <c r="C39" s="83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="93"/>
       <c r="E39" s="93"/>
       <c r="F39" s="93"/>
       <c r="G39" s="94"/>
       <c r="H39" s="12" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="18" customHeight="1">
@@ -6053,7 +6075,7 @@
       <c r="F40" s="93"/>
       <c r="G40" s="94"/>
       <c r="H40" s="12" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="18" customHeight="1">
@@ -7947,7 +7969,7 @@
     </row>
     <row r="214" spans="2:8" ht="15.75" customHeight="1">
       <c r="B214" s="34" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C214" s="34"/>
       <c r="D214" s="34" t="s">
@@ -8926,7 +8948,7 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -11383,7 +11405,7 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="D13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -14038,9 +14060,9 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="D3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14242,13 +14264,13 @@
         <v>86</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H11" s="13">
         <v>3</v>
       </c>
       <c r="I11" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="37"/>
       <c r="K11" s="2">
@@ -14281,13 +14303,13 @@
         <v>97</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H12" s="13">
         <v>2</v>
       </c>
       <c r="I12" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="17"/>
       <c r="K12" s="2">
@@ -14310,13 +14332,13 @@
         <v>101</v>
       </c>
       <c r="G13" s="43" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H13" s="13">
         <v>2</v>
       </c>
       <c r="I13" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="37"/>
       <c r="K13" s="2">
@@ -14339,13 +14361,13 @@
         <v>84</v>
       </c>
       <c r="G14" s="43" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H14" s="13">
         <v>2</v>
       </c>
       <c r="I14" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="37"/>
       <c r="K14" s="2">
@@ -14368,13 +14390,13 @@
         <v>101</v>
       </c>
       <c r="G15" s="43" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H15" s="13">
         <v>16</v>
       </c>
       <c r="I15" s="13">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J15" s="37"/>
       <c r="K15" s="2"/>
@@ -14394,13 +14416,13 @@
         <v>97</v>
       </c>
       <c r="G16" s="43" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H16" s="13">
         <v>16</v>
       </c>
       <c r="I16" s="13">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J16" s="37"/>
       <c r="K16" s="2"/>
@@ -14420,13 +14442,13 @@
         <v>84</v>
       </c>
       <c r="G17" s="43" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H17" s="13">
         <v>14</v>
       </c>
       <c r="I17" s="13">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J17" s="37"/>
       <c r="K17" s="2"/>
@@ -14446,13 +14468,13 @@
         <v>86</v>
       </c>
       <c r="G18" s="43" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H18" s="13">
         <v>24</v>
       </c>
       <c r="I18" s="13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J18" s="37"/>
       <c r="K18" s="2"/>
@@ -15184,7 +15206,7 @@
       </c>
       <c r="I61" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="2:10" ht="15.75" customHeight="1">
@@ -15198,7 +15220,7 @@
       <c r="F62" s="30"/>
       <c r="G62" s="30">
         <f>COUNTIFS(G11:G60, "Concluído",D11:D60, "&lt;&gt;"&amp;"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="2:10" ht="15.75" customHeight="1">
@@ -16658,9 +16680,9 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -16851,12 +16873,20 @@
         <v>1</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="43"/>
+      <c r="D11" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="11">
+        <v>19</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H11" s="13">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I11" s="13">
         <v>0</v>
@@ -16882,12 +16912,20 @@
         <v>2</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="43"/>
+      <c r="D12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="11">
+        <v>18</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H12" s="13">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I12" s="13">
         <v>0</v>
@@ -16903,12 +16941,20 @@
         <v>3</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="43"/>
+      <c r="D13" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H13" s="13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I13" s="13">
         <v>0</v>
@@ -16924,12 +16970,20 @@
         <v>4</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="43"/>
+      <c r="D14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H14" s="13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I14" s="13">
         <v>0</v>
@@ -16945,12 +16999,20 @@
         <v>5</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="43"/>
+      <c r="D15" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H15" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="13">
         <v>0</v>
@@ -16966,12 +17028,20 @@
         <v>6</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="43"/>
+      <c r="D16" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H16" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="13">
         <v>0</v>
@@ -16987,12 +17057,20 @@
         <v>7</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="43"/>
+      <c r="D17" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H17" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I17" s="13">
         <v>0</v>
@@ -17008,12 +17086,20 @@
         <v>8</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="43"/>
+      <c r="D18" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H18" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="13">
         <v>0</v>
@@ -17763,7 +17849,7 @@
       </c>
       <c r="H61" s="32">
         <f t="shared" ref="H61:I61" si="1">SUM(H11:H60)</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="I61" s="32">
         <f t="shared" si="1"/>
@@ -17775,7 +17861,7 @@
       <c r="C62" s="30"/>
       <c r="D62" s="30">
         <f>COUNTIFS(D11:D60, "&lt;&gt;"&amp;"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E62" s="30"/>
       <c r="F62" s="30"/>
@@ -19101,7 +19187,7 @@
   <dimension ref="A1:U1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="B11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -21660,7 +21746,7 @@
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1">
       <c r="B9" s="85" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>

</xml_diff>

<commit_message>
[Update] atualização do planejamento sprint
</commit_message>
<xml_diff>
--- a/Artefatos/planejamento-sprints.xlsx
+++ b/Artefatos/planejamento-sprints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sgapucminasbr-my.sharepoint.com/personal/1349196_sga_pucminas_br/Documents/git/plf-es-2022-2-ti3-6653100-sistema-atelier-picinin/Artefatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{12CFFE64-A39B-4D05-AE8D-0E79864B7B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="14_{12CFFE64-A39B-4D05-AE8D-0E79864B7B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B52B2A1-27B9-49CC-A20F-302DD2D72552}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados do Projeto" sheetId="1" r:id="rId1"/>
@@ -376,7 +376,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="128">
   <si>
     <t>PONTIFÍCIA UNIVERSIDADE CATÓLICA DE MINAS GERAIS</t>
   </si>
@@ -785,6 +785,12 @@
   </si>
   <si>
     <t>Diagrama de casos de uso</t>
+  </si>
+  <si>
+    <t>Diagrama de classes</t>
+  </si>
+  <si>
+    <t>Descrição caso de uso</t>
   </si>
 </sst>
 </file>
@@ -1360,6 +1366,37 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1368,7 +1405,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1376,41 +1412,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1427,8 +1430,14 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1438,9 +1447,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4029,139 +4035,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="66"/>
+      <c r="B1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="81"/>
     </row>
     <row r="2" spans="2:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="83"/>
     </row>
     <row r="3" spans="2:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="69"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="83"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="73"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="75"/>
     </row>
     <row r="6" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="76"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="2:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B9" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="76"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
       <c r="F9" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="75"/>
-      <c r="H9" s="76"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="69"/>
     </row>
     <row r="10" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="76"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="69"/>
     </row>
     <row r="11" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="76"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="69"/>
     </row>
     <row r="12" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="76"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="69"/>
     </row>
     <row r="13" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="76"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="69"/>
       <c r="I13" s="16"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="79"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="76"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="69"/>
     </row>
     <row r="15" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E15" s="18"/>
@@ -4263,16 +4269,16 @@
     <row r="98" spans="1:15" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="50"/>
-      <c r="B99" s="81"/>
-      <c r="C99" s="68"/>
-      <c r="D99" s="82" t="s">
+      <c r="B99" s="71"/>
+      <c r="C99" s="66"/>
+      <c r="D99" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="E99" s="68"/>
-      <c r="F99" s="82" t="s">
+      <c r="E99" s="66"/>
+      <c r="F99" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="G99" s="68"/>
+      <c r="G99" s="66"/>
       <c r="H99" s="51" t="s">
         <v>15</v>
       </c>
@@ -4294,12 +4300,12 @@
     </row>
     <row r="100" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A100" s="50"/>
-      <c r="B100" s="84"/>
-      <c r="C100" s="68"/>
-      <c r="D100" s="83" t="s">
+      <c r="B100" s="65"/>
+      <c r="C100" s="66"/>
+      <c r="D100" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="E100" s="68"/>
+      <c r="E100" s="66"/>
       <c r="F100" s="53" t="s">
         <v>21</v>
       </c>
@@ -4333,12 +4339,12 @@
     </row>
     <row r="101" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="50"/>
-      <c r="B101" s="84"/>
-      <c r="C101" s="68"/>
-      <c r="D101" s="83" t="s">
+      <c r="B101" s="65"/>
+      <c r="C101" s="66"/>
+      <c r="D101" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="E101" s="68"/>
+      <c r="E101" s="66"/>
       <c r="F101" s="53" t="s">
         <v>26</v>
       </c>
@@ -4372,12 +4378,12 @@
     </row>
     <row r="102" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A102" s="50"/>
-      <c r="B102" s="84"/>
-      <c r="C102" s="68"/>
-      <c r="D102" s="83" t="s">
+      <c r="B102" s="65"/>
+      <c r="C102" s="66"/>
+      <c r="D102" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="E102" s="68"/>
+      <c r="E102" s="66"/>
       <c r="F102" s="53"/>
       <c r="G102" s="54" t="s">
         <v>31</v>
@@ -4409,12 +4415,12 @@
     </row>
     <row r="103" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="50"/>
-      <c r="B103" s="84"/>
-      <c r="C103" s="68"/>
-      <c r="D103" s="83" t="s">
+      <c r="B103" s="65"/>
+      <c r="C103" s="66"/>
+      <c r="D103" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="E103" s="68"/>
+      <c r="E103" s="66"/>
       <c r="F103" s="53"/>
       <c r="G103" s="54" t="s">
         <v>34</v>
@@ -4444,12 +4450,12 @@
     </row>
     <row r="104" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="50"/>
-      <c r="B104" s="84"/>
-      <c r="C104" s="68"/>
-      <c r="D104" s="83" t="s">
+      <c r="B104" s="65"/>
+      <c r="C104" s="66"/>
+      <c r="D104" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="E104" s="68"/>
+      <c r="E104" s="66"/>
       <c r="F104" s="53"/>
       <c r="G104" s="54" t="s">
         <v>37</v>
@@ -4474,8 +4480,8 @@
     </row>
     <row r="105" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="50"/>
-      <c r="B105" s="84"/>
-      <c r="C105" s="68"/>
+      <c r="B105" s="65"/>
+      <c r="C105" s="66"/>
       <c r="F105" s="53"/>
       <c r="G105" s="54" t="s">
         <v>38</v>
@@ -4488,8 +4494,8 @@
     </row>
     <row r="106" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="50"/>
-      <c r="B106" s="84"/>
-      <c r="C106" s="68"/>
+      <c r="B106" s="65"/>
+      <c r="C106" s="66"/>
       <c r="D106" s="56"/>
       <c r="E106" s="53"/>
       <c r="F106" s="53"/>
@@ -5457,12 +5463,22 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="B99:C99"/>
     <mergeCell ref="D99:E99"/>
@@ -5474,22 +5490,12 @@
     <mergeCell ref="B102:C102"/>
     <mergeCell ref="D102:E102"/>
     <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="D104:E104"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="F10:F14" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -5533,59 +5539,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="66"/>
+      <c r="B1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="81"/>
     </row>
     <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="83"/>
     </row>
     <row r="3" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="69"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="83"/>
     </row>
     <row r="4" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="73"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="75"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
@@ -5597,16 +5603,16 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" ht="26.25" x14ac:dyDescent="0.2">
-      <c r="B7" s="85" t="str">
+      <c r="B7" s="92" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Sistema Atelier Picinin</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="76"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
@@ -5618,15 +5624,15 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="76"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="69"/>
     </row>
     <row r="10" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
@@ -5638,11 +5644,11 @@
       <c r="D10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="87" t="s">
+      <c r="E10" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="75"/>
-      <c r="G10" s="76"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="6" t="s">
         <v>44</v>
       </c>
@@ -5658,11 +5664,11 @@
         <f>C11+13</f>
         <v>44809</v>
       </c>
-      <c r="E11" s="88" t="s">
+      <c r="E11" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="75"/>
-      <c r="G11" s="76"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="15" t="s">
         <v>46</v>
       </c>
@@ -5679,9 +5685,9 @@
         <f t="shared" ref="D12" si="1">C12+13</f>
         <v>44823</v>
       </c>
-      <c r="E12" s="88"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5696,9 +5702,9 @@
         <f>C13+13</f>
         <v>44837</v>
       </c>
-      <c r="E13" s="88"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="76"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="69"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5713,9 +5719,9 @@
         <f>C14+20</f>
         <v>44858</v>
       </c>
-      <c r="E14" s="89"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5747,9 +5753,9 @@
         <f>C16+13</f>
         <v>44886</v>
       </c>
-      <c r="E16" s="89"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
       <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5772,13 +5778,13 @@
     </row>
     <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="20"/>
-      <c r="C19" s="90" t="s">
+      <c r="C19" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
       <c r="H19" s="22" t="s">
         <v>48</v>
       </c>
@@ -5787,11 +5793,11 @@
       <c r="B20" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="76"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="69"/>
       <c r="H20" s="25" t="s">
         <v>49</v>
       </c>
@@ -5801,11 +5807,11 @@
       <c r="B21" s="27">
         <v>0</v>
       </c>
-      <c r="C21" s="92"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="76"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="69"/>
       <c r="H21" s="28"/>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
@@ -5822,13 +5828,13 @@
       <c r="B22" s="9">
         <v>1</v>
       </c>
-      <c r="C22" s="93" t="s">
+      <c r="C22" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="76"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="69"/>
       <c r="H22" s="12" t="s">
         <v>51</v>
       </c>
@@ -5837,13 +5843,13 @@
       <c r="B23" s="27">
         <v>2</v>
       </c>
-      <c r="C23" s="93" t="s">
+      <c r="C23" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="76"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="69"/>
       <c r="H23" s="12" t="s">
         <v>51</v>
       </c>
@@ -5852,13 +5858,13 @@
       <c r="B24" s="9">
         <v>3</v>
       </c>
-      <c r="C24" s="93" t="s">
+      <c r="C24" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="76"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="69"/>
       <c r="H24" s="12" t="s">
         <v>51</v>
       </c>
@@ -5867,13 +5873,13 @@
       <c r="B25" s="27">
         <v>4</v>
       </c>
-      <c r="C25" s="93" t="s">
+      <c r="C25" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="76"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="69"/>
       <c r="H25" s="12" t="s">
         <v>51</v>
       </c>
@@ -5882,13 +5888,13 @@
       <c r="B26" s="9">
         <v>5</v>
       </c>
-      <c r="C26" s="93" t="s">
+      <c r="C26" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="76"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="69"/>
       <c r="H26" s="12" t="s">
         <v>51</v>
       </c>
@@ -5897,13 +5903,13 @@
       <c r="B27" s="27">
         <v>6</v>
       </c>
-      <c r="C27" s="93" t="s">
+      <c r="C27" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="76"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="69"/>
       <c r="H27" s="12" t="s">
         <v>51</v>
       </c>
@@ -5912,13 +5918,13 @@
       <c r="B28" s="9">
         <v>7</v>
       </c>
-      <c r="C28" s="93" t="s">
+      <c r="C28" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="76"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="69"/>
       <c r="H28" s="12" t="s">
         <v>70</v>
       </c>
@@ -5927,13 +5933,13 @@
       <c r="B29" s="27">
         <v>8</v>
       </c>
-      <c r="C29" s="93" t="s">
+      <c r="C29" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="69"/>
       <c r="H29" s="12" t="s">
         <v>58</v>
       </c>
@@ -5942,13 +5948,13 @@
       <c r="B30" s="9">
         <v>9</v>
       </c>
-      <c r="C30" s="93" t="s">
+      <c r="C30" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="76"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="69"/>
       <c r="H30" s="12" t="s">
         <v>70</v>
       </c>
@@ -5957,13 +5963,13 @@
       <c r="B31" s="27">
         <v>10</v>
       </c>
-      <c r="C31" s="93" t="s">
+      <c r="C31" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="76"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="69"/>
       <c r="H31" s="12" t="s">
         <v>51</v>
       </c>
@@ -5972,13 +5978,13 @@
       <c r="B32" s="9">
         <v>11</v>
       </c>
-      <c r="C32" s="93" t="s">
+      <c r="C32" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="76"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="69"/>
       <c r="H32" s="12" t="s">
         <v>51</v>
       </c>
@@ -5987,13 +5993,13 @@
       <c r="B33" s="27">
         <v>12</v>
       </c>
-      <c r="C33" s="93" t="s">
+      <c r="C33" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="76"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="69"/>
       <c r="H33" s="12" t="s">
         <v>51</v>
       </c>
@@ -6002,13 +6008,13 @@
       <c r="B34" s="9">
         <v>13</v>
       </c>
-      <c r="C34" s="93" t="s">
+      <c r="C34" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="76"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="69"/>
       <c r="H34" s="12" t="s">
         <v>51</v>
       </c>
@@ -6017,13 +6023,13 @@
       <c r="B35" s="27">
         <v>14</v>
       </c>
-      <c r="C35" s="93" t="s">
+      <c r="C35" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="69"/>
       <c r="H35" s="12" t="s">
         <v>51</v>
       </c>
@@ -6032,13 +6038,13 @@
       <c r="B36" s="9">
         <v>15</v>
       </c>
-      <c r="C36" s="93" t="s">
+      <c r="C36" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="76"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="69"/>
       <c r="H36" s="12" t="s">
         <v>51</v>
       </c>
@@ -6047,13 +6053,13 @@
       <c r="B37" s="27">
         <v>16</v>
       </c>
-      <c r="C37" s="93" t="s">
+      <c r="C37" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="76"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="68"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="69"/>
       <c r="H37" s="12" t="s">
         <v>51</v>
       </c>
@@ -6062,13 +6068,13 @@
       <c r="B38" s="9">
         <v>17</v>
       </c>
-      <c r="C38" s="93" t="s">
+      <c r="C38" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="76"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="69"/>
       <c r="H38" s="12" t="s">
         <v>58</v>
       </c>
@@ -6077,13 +6083,13 @@
       <c r="B39" s="27">
         <v>18</v>
       </c>
-      <c r="C39" s="93" t="s">
+      <c r="C39" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="75"/>
-      <c r="E39" s="75"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="76"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="68"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="69"/>
       <c r="H39" s="12" t="s">
         <v>51</v>
       </c>
@@ -6092,13 +6098,13 @@
       <c r="B40" s="9">
         <v>19</v>
       </c>
-      <c r="C40" s="93" t="s">
+      <c r="C40" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="76"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="69"/>
       <c r="H40" s="12" t="s">
         <v>51</v>
       </c>
@@ -6107,11 +6113,11 @@
       <c r="B41" s="27">
         <v>20</v>
       </c>
-      <c r="C41" s="93"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="76"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="69"/>
       <c r="H41" s="12" t="s">
         <v>58</v>
       </c>
@@ -6120,11 +6126,11 @@
       <c r="B42" s="9">
         <v>21</v>
       </c>
-      <c r="C42" s="93"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="76"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="69"/>
       <c r="H42" s="12" t="s">
         <v>58</v>
       </c>
@@ -6133,11 +6139,11 @@
       <c r="B43" s="27">
         <v>22</v>
       </c>
-      <c r="C43" s="93"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="75"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="76"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="69"/>
       <c r="H43" s="12" t="s">
         <v>58</v>
       </c>
@@ -6146,11 +6152,11 @@
       <c r="B44" s="9">
         <v>23</v>
       </c>
-      <c r="C44" s="93"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="76"/>
+      <c r="C44" s="86"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="69"/>
       <c r="H44" s="12" t="s">
         <v>58</v>
       </c>
@@ -6159,11 +6165,11 @@
       <c r="B45" s="27">
         <v>24</v>
       </c>
-      <c r="C45" s="93"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="76"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="69"/>
       <c r="H45" s="12" t="s">
         <v>58</v>
       </c>
@@ -6172,11 +6178,11 @@
       <c r="B46" s="9">
         <v>25</v>
       </c>
-      <c r="C46" s="93"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="76"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="68"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="69"/>
       <c r="H46" s="12" t="s">
         <v>58</v>
       </c>
@@ -6185,11 +6191,11 @@
       <c r="B47" s="27">
         <v>26</v>
       </c>
-      <c r="C47" s="93"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="76"/>
+      <c r="C47" s="86"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="68"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="69"/>
       <c r="H47" s="12" t="s">
         <v>58</v>
       </c>
@@ -6198,11 +6204,11 @@
       <c r="B48" s="9">
         <v>27</v>
       </c>
-      <c r="C48" s="93"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="75"/>
-      <c r="G48" s="76"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="68"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="69"/>
       <c r="H48" s="12" t="s">
         <v>58</v>
       </c>
@@ -6211,11 +6217,11 @@
       <c r="B49" s="27">
         <v>28</v>
       </c>
-      <c r="C49" s="93"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="76"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="68"/>
+      <c r="F49" s="68"/>
+      <c r="G49" s="69"/>
       <c r="H49" s="12" t="s">
         <v>58</v>
       </c>
@@ -6224,11 +6230,11 @@
       <c r="B50" s="9">
         <v>29</v>
       </c>
-      <c r="C50" s="93"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="76"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="68"/>
+      <c r="E50" s="68"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="69"/>
       <c r="H50" s="12" t="s">
         <v>58</v>
       </c>
@@ -6237,11 +6243,11 @@
       <c r="B51" s="27">
         <v>30</v>
       </c>
-      <c r="C51" s="93"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="76"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="68"/>
+      <c r="G51" s="69"/>
       <c r="H51" s="12" t="s">
         <v>58</v>
       </c>
@@ -6250,11 +6256,11 @@
       <c r="B52" s="9">
         <v>31</v>
       </c>
-      <c r="C52" s="93"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="76"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="68"/>
+      <c r="E52" s="68"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="69"/>
       <c r="H52" s="12" t="s">
         <v>58</v>
       </c>
@@ -6263,11 +6269,11 @@
       <c r="B53" s="27">
         <v>32</v>
       </c>
-      <c r="C53" s="93"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="76"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="68"/>
+      <c r="E53" s="68"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="69"/>
       <c r="H53" s="12" t="s">
         <v>58</v>
       </c>
@@ -6276,11 +6282,11 @@
       <c r="B54" s="9">
         <v>33</v>
       </c>
-      <c r="C54" s="93"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="75"/>
-      <c r="G54" s="76"/>
+      <c r="C54" s="86"/>
+      <c r="D54" s="68"/>
+      <c r="E54" s="68"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="69"/>
       <c r="H54" s="12" t="s">
         <v>58</v>
       </c>
@@ -6289,11 +6295,11 @@
       <c r="B55" s="27">
         <v>34</v>
       </c>
-      <c r="C55" s="93"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="76"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="68"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="69"/>
       <c r="H55" s="12" t="s">
         <v>58</v>
       </c>
@@ -6302,11 +6308,11 @@
       <c r="B56" s="9">
         <v>35</v>
       </c>
-      <c r="C56" s="93"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="76"/>
+      <c r="C56" s="86"/>
+      <c r="D56" s="68"/>
+      <c r="E56" s="68"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="69"/>
       <c r="H56" s="12" t="s">
         <v>58</v>
       </c>
@@ -6315,11 +6321,11 @@
       <c r="B57" s="27">
         <v>36</v>
       </c>
-      <c r="C57" s="93"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="76"/>
+      <c r="C57" s="86"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="68"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="69"/>
       <c r="H57" s="12" t="s">
         <v>58</v>
       </c>
@@ -6328,11 +6334,11 @@
       <c r="B58" s="9">
         <v>37</v>
       </c>
-      <c r="C58" s="93"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="76"/>
+      <c r="C58" s="86"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="68"/>
+      <c r="F58" s="68"/>
+      <c r="G58" s="69"/>
       <c r="H58" s="12" t="s">
         <v>58</v>
       </c>
@@ -6341,11 +6347,11 @@
       <c r="B59" s="27">
         <v>38</v>
       </c>
-      <c r="C59" s="93"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="75"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="76"/>
+      <c r="C59" s="86"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="68"/>
+      <c r="F59" s="68"/>
+      <c r="G59" s="69"/>
       <c r="H59" s="12" t="s">
         <v>58</v>
       </c>
@@ -6354,11 +6360,11 @@
       <c r="B60" s="9">
         <v>39</v>
       </c>
-      <c r="C60" s="93"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="75"/>
-      <c r="F60" s="75"/>
-      <c r="G60" s="76"/>
+      <c r="C60" s="86"/>
+      <c r="D60" s="68"/>
+      <c r="E60" s="68"/>
+      <c r="F60" s="68"/>
+      <c r="G60" s="69"/>
       <c r="H60" s="12" t="s">
         <v>58</v>
       </c>
@@ -6367,11 +6373,11 @@
       <c r="B61" s="27">
         <v>40</v>
       </c>
-      <c r="C61" s="93"/>
-      <c r="D61" s="75"/>
-      <c r="E61" s="75"/>
-      <c r="F61" s="75"/>
-      <c r="G61" s="76"/>
+      <c r="C61" s="86"/>
+      <c r="D61" s="68"/>
+      <c r="E61" s="68"/>
+      <c r="F61" s="68"/>
+      <c r="G61" s="69"/>
       <c r="H61" s="12" t="s">
         <v>58</v>
       </c>
@@ -6380,11 +6386,11 @@
       <c r="B62" s="9">
         <v>41</v>
       </c>
-      <c r="C62" s="93"/>
-      <c r="D62" s="75"/>
-      <c r="E62" s="75"/>
-      <c r="F62" s="75"/>
-      <c r="G62" s="76"/>
+      <c r="C62" s="86"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="68"/>
+      <c r="F62" s="68"/>
+      <c r="G62" s="69"/>
       <c r="H62" s="12" t="s">
         <v>58</v>
       </c>
@@ -6393,11 +6399,11 @@
       <c r="B63" s="27">
         <v>42</v>
       </c>
-      <c r="C63" s="93"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="76"/>
+      <c r="C63" s="86"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="68"/>
+      <c r="G63" s="69"/>
       <c r="H63" s="12" t="s">
         <v>58</v>
       </c>
@@ -6406,11 +6412,11 @@
       <c r="B64" s="9">
         <v>43</v>
       </c>
-      <c r="C64" s="93"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="76"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="68"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="69"/>
       <c r="H64" s="12" t="s">
         <v>58</v>
       </c>
@@ -6419,11 +6425,11 @@
       <c r="B65" s="27">
         <v>44</v>
       </c>
-      <c r="C65" s="93"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="76"/>
+      <c r="C65" s="86"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="69"/>
       <c r="H65" s="12" t="s">
         <v>58</v>
       </c>
@@ -6432,11 +6438,11 @@
       <c r="B66" s="9">
         <v>45</v>
       </c>
-      <c r="C66" s="93"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="76"/>
+      <c r="C66" s="86"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="69"/>
       <c r="H66" s="12" t="s">
         <v>58</v>
       </c>
@@ -6445,11 +6451,11 @@
       <c r="B67" s="27">
         <v>46</v>
       </c>
-      <c r="C67" s="93"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="76"/>
+      <c r="C67" s="86"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="69"/>
       <c r="H67" s="12" t="s">
         <v>58</v>
       </c>
@@ -6458,11 +6464,11 @@
       <c r="B68" s="9">
         <v>47</v>
       </c>
-      <c r="C68" s="93"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="76"/>
+      <c r="C68" s="86"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="69"/>
       <c r="H68" s="12" t="s">
         <v>58</v>
       </c>
@@ -6471,11 +6477,11 @@
       <c r="B69" s="27">
         <v>48</v>
       </c>
-      <c r="C69" s="93"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="76"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="69"/>
       <c r="H69" s="12" t="s">
         <v>58</v>
       </c>
@@ -6484,11 +6490,11 @@
       <c r="B70" s="9">
         <v>49</v>
       </c>
-      <c r="C70" s="93"/>
-      <c r="D70" s="75"/>
-      <c r="E70" s="75"/>
-      <c r="F70" s="75"/>
-      <c r="G70" s="76"/>
+      <c r="C70" s="86"/>
+      <c r="D70" s="68"/>
+      <c r="E70" s="68"/>
+      <c r="F70" s="68"/>
+      <c r="G70" s="69"/>
       <c r="H70" s="12" t="s">
         <v>58</v>
       </c>
@@ -6497,11 +6503,11 @@
       <c r="B71" s="27">
         <v>50</v>
       </c>
-      <c r="C71" s="93"/>
-      <c r="D71" s="75"/>
-      <c r="E71" s="75"/>
-      <c r="F71" s="75"/>
-      <c r="G71" s="76"/>
+      <c r="C71" s="86"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="68"/>
+      <c r="F71" s="68"/>
+      <c r="G71" s="69"/>
       <c r="H71" s="12" t="s">
         <v>58</v>
       </c>
@@ -6510,11 +6516,11 @@
       <c r="B72" s="9">
         <v>51</v>
       </c>
-      <c r="C72" s="93"/>
-      <c r="D72" s="75"/>
-      <c r="E72" s="75"/>
-      <c r="F72" s="75"/>
-      <c r="G72" s="76"/>
+      <c r="C72" s="86"/>
+      <c r="D72" s="68"/>
+      <c r="E72" s="68"/>
+      <c r="F72" s="68"/>
+      <c r="G72" s="69"/>
       <c r="H72" s="12" t="s">
         <v>58</v>
       </c>
@@ -6523,11 +6529,11 @@
       <c r="B73" s="27">
         <v>52</v>
       </c>
-      <c r="C73" s="93"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
-      <c r="G73" s="76"/>
+      <c r="C73" s="86"/>
+      <c r="D73" s="68"/>
+      <c r="E73" s="68"/>
+      <c r="F73" s="68"/>
+      <c r="G73" s="69"/>
       <c r="H73" s="12" t="s">
         <v>58</v>
       </c>
@@ -6536,11 +6542,11 @@
       <c r="B74" s="9">
         <v>53</v>
       </c>
-      <c r="C74" s="93"/>
-      <c r="D74" s="75"/>
-      <c r="E74" s="75"/>
-      <c r="F74" s="75"/>
-      <c r="G74" s="76"/>
+      <c r="C74" s="86"/>
+      <c r="D74" s="68"/>
+      <c r="E74" s="68"/>
+      <c r="F74" s="68"/>
+      <c r="G74" s="69"/>
       <c r="H74" s="12" t="s">
         <v>58</v>
       </c>
@@ -6549,11 +6555,11 @@
       <c r="B75" s="27">
         <v>54</v>
       </c>
-      <c r="C75" s="93"/>
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
-      <c r="F75" s="75"/>
-      <c r="G75" s="76"/>
+      <c r="C75" s="86"/>
+      <c r="D75" s="68"/>
+      <c r="E75" s="68"/>
+      <c r="F75" s="68"/>
+      <c r="G75" s="69"/>
       <c r="H75" s="12" t="s">
         <v>58</v>
       </c>
@@ -6562,11 +6568,11 @@
       <c r="B76" s="9">
         <v>55</v>
       </c>
-      <c r="C76" s="93"/>
-      <c r="D76" s="75"/>
-      <c r="E76" s="75"/>
-      <c r="F76" s="75"/>
-      <c r="G76" s="76"/>
+      <c r="C76" s="86"/>
+      <c r="D76" s="68"/>
+      <c r="E76" s="68"/>
+      <c r="F76" s="68"/>
+      <c r="G76" s="69"/>
       <c r="H76" s="12" t="s">
         <v>58</v>
       </c>
@@ -6575,11 +6581,11 @@
       <c r="B77" s="27">
         <v>56</v>
       </c>
-      <c r="C77" s="93"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
-      <c r="F77" s="75"/>
-      <c r="G77" s="76"/>
+      <c r="C77" s="86"/>
+      <c r="D77" s="68"/>
+      <c r="E77" s="68"/>
+      <c r="F77" s="68"/>
+      <c r="G77" s="69"/>
       <c r="H77" s="12" t="s">
         <v>58</v>
       </c>
@@ -6588,11 +6594,11 @@
       <c r="B78" s="9">
         <v>57</v>
       </c>
-      <c r="C78" s="93"/>
-      <c r="D78" s="75"/>
-      <c r="E78" s="75"/>
-      <c r="F78" s="75"/>
-      <c r="G78" s="76"/>
+      <c r="C78" s="86"/>
+      <c r="D78" s="68"/>
+      <c r="E78" s="68"/>
+      <c r="F78" s="68"/>
+      <c r="G78" s="69"/>
       <c r="H78" s="12" t="s">
         <v>58</v>
       </c>
@@ -6601,11 +6607,11 @@
       <c r="B79" s="27">
         <v>58</v>
       </c>
-      <c r="C79" s="93"/>
-      <c r="D79" s="75"/>
-      <c r="E79" s="75"/>
-      <c r="F79" s="75"/>
-      <c r="G79" s="76"/>
+      <c r="C79" s="86"/>
+      <c r="D79" s="68"/>
+      <c r="E79" s="68"/>
+      <c r="F79" s="68"/>
+      <c r="G79" s="69"/>
       <c r="H79" s="12" t="s">
         <v>58</v>
       </c>
@@ -6614,11 +6620,11 @@
       <c r="B80" s="9">
         <v>59</v>
       </c>
-      <c r="C80" s="93"/>
-      <c r="D80" s="75"/>
-      <c r="E80" s="75"/>
-      <c r="F80" s="75"/>
-      <c r="G80" s="76"/>
+      <c r="C80" s="86"/>
+      <c r="D80" s="68"/>
+      <c r="E80" s="68"/>
+      <c r="F80" s="68"/>
+      <c r="G80" s="69"/>
       <c r="H80" s="12" t="s">
         <v>58</v>
       </c>
@@ -6627,11 +6633,11 @@
       <c r="B81" s="27">
         <v>60</v>
       </c>
-      <c r="C81" s="93"/>
-      <c r="D81" s="75"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="75"/>
-      <c r="G81" s="76"/>
+      <c r="C81" s="86"/>
+      <c r="D81" s="68"/>
+      <c r="E81" s="68"/>
+      <c r="F81" s="68"/>
+      <c r="G81" s="69"/>
       <c r="H81" s="12" t="s">
         <v>58</v>
       </c>
@@ -6640,11 +6646,11 @@
       <c r="B82" s="9">
         <v>61</v>
       </c>
-      <c r="C82" s="93"/>
-      <c r="D82" s="75"/>
-      <c r="E82" s="75"/>
-      <c r="F82" s="75"/>
-      <c r="G82" s="76"/>
+      <c r="C82" s="86"/>
+      <c r="D82" s="68"/>
+      <c r="E82" s="68"/>
+      <c r="F82" s="68"/>
+      <c r="G82" s="69"/>
       <c r="H82" s="12" t="s">
         <v>58</v>
       </c>
@@ -6653,11 +6659,11 @@
       <c r="B83" s="27">
         <v>62</v>
       </c>
-      <c r="C83" s="93"/>
-      <c r="D83" s="75"/>
-      <c r="E83" s="75"/>
-      <c r="F83" s="75"/>
-      <c r="G83" s="76"/>
+      <c r="C83" s="86"/>
+      <c r="D83" s="68"/>
+      <c r="E83" s="68"/>
+      <c r="F83" s="68"/>
+      <c r="G83" s="69"/>
       <c r="H83" s="12" t="s">
         <v>58</v>
       </c>
@@ -6666,11 +6672,11 @@
       <c r="B84" s="9">
         <v>63</v>
       </c>
-      <c r="C84" s="93"/>
-      <c r="D84" s="75"/>
-      <c r="E84" s="75"/>
-      <c r="F84" s="75"/>
-      <c r="G84" s="76"/>
+      <c r="C84" s="86"/>
+      <c r="D84" s="68"/>
+      <c r="E84" s="68"/>
+      <c r="F84" s="68"/>
+      <c r="G84" s="69"/>
       <c r="H84" s="12" t="s">
         <v>58</v>
       </c>
@@ -6679,11 +6685,11 @@
       <c r="B85" s="27">
         <v>64</v>
       </c>
-      <c r="C85" s="93"/>
-      <c r="D85" s="75"/>
-      <c r="E85" s="75"/>
-      <c r="F85" s="75"/>
-      <c r="G85" s="76"/>
+      <c r="C85" s="86"/>
+      <c r="D85" s="68"/>
+      <c r="E85" s="68"/>
+      <c r="F85" s="68"/>
+      <c r="G85" s="69"/>
       <c r="H85" s="12" t="s">
         <v>58</v>
       </c>
@@ -6692,11 +6698,11 @@
       <c r="B86" s="9">
         <v>65</v>
       </c>
-      <c r="C86" s="93"/>
-      <c r="D86" s="75"/>
-      <c r="E86" s="75"/>
-      <c r="F86" s="75"/>
-      <c r="G86" s="76"/>
+      <c r="C86" s="86"/>
+      <c r="D86" s="68"/>
+      <c r="E86" s="68"/>
+      <c r="F86" s="68"/>
+      <c r="G86" s="69"/>
       <c r="H86" s="12" t="s">
         <v>58</v>
       </c>
@@ -6705,11 +6711,11 @@
       <c r="B87" s="27">
         <v>66</v>
       </c>
-      <c r="C87" s="93"/>
-      <c r="D87" s="75"/>
-      <c r="E87" s="75"/>
-      <c r="F87" s="75"/>
-      <c r="G87" s="76"/>
+      <c r="C87" s="86"/>
+      <c r="D87" s="68"/>
+      <c r="E87" s="68"/>
+      <c r="F87" s="68"/>
+      <c r="G87" s="69"/>
       <c r="H87" s="12" t="s">
         <v>58</v>
       </c>
@@ -6718,11 +6724,11 @@
       <c r="B88" s="9">
         <v>67</v>
       </c>
-      <c r="C88" s="93"/>
-      <c r="D88" s="75"/>
-      <c r="E88" s="75"/>
-      <c r="F88" s="75"/>
-      <c r="G88" s="76"/>
+      <c r="C88" s="86"/>
+      <c r="D88" s="68"/>
+      <c r="E88" s="68"/>
+      <c r="F88" s="68"/>
+      <c r="G88" s="69"/>
       <c r="H88" s="12" t="s">
         <v>58</v>
       </c>
@@ -6731,11 +6737,11 @@
       <c r="B89" s="27">
         <v>68</v>
       </c>
-      <c r="C89" s="93"/>
-      <c r="D89" s="75"/>
-      <c r="E89" s="75"/>
-      <c r="F89" s="75"/>
-      <c r="G89" s="76"/>
+      <c r="C89" s="86"/>
+      <c r="D89" s="68"/>
+      <c r="E89" s="68"/>
+      <c r="F89" s="68"/>
+      <c r="G89" s="69"/>
       <c r="H89" s="12" t="s">
         <v>58</v>
       </c>
@@ -6744,11 +6750,11 @@
       <c r="B90" s="9">
         <v>69</v>
       </c>
-      <c r="C90" s="93"/>
-      <c r="D90" s="75"/>
-      <c r="E90" s="75"/>
-      <c r="F90" s="75"/>
-      <c r="G90" s="76"/>
+      <c r="C90" s="86"/>
+      <c r="D90" s="68"/>
+      <c r="E90" s="68"/>
+      <c r="F90" s="68"/>
+      <c r="G90" s="69"/>
       <c r="H90" s="12" t="s">
         <v>58</v>
       </c>
@@ -6757,11 +6763,11 @@
       <c r="B91" s="27">
         <v>70</v>
       </c>
-      <c r="C91" s="93"/>
-      <c r="D91" s="75"/>
-      <c r="E91" s="75"/>
-      <c r="F91" s="75"/>
-      <c r="G91" s="76"/>
+      <c r="C91" s="86"/>
+      <c r="D91" s="68"/>
+      <c r="E91" s="68"/>
+      <c r="F91" s="68"/>
+      <c r="G91" s="69"/>
       <c r="H91" s="12" t="s">
         <v>58</v>
       </c>
@@ -6770,11 +6776,11 @@
       <c r="B92" s="9">
         <v>71</v>
       </c>
-      <c r="C92" s="93"/>
-      <c r="D92" s="75"/>
-      <c r="E92" s="75"/>
-      <c r="F92" s="75"/>
-      <c r="G92" s="76"/>
+      <c r="C92" s="86"/>
+      <c r="D92" s="68"/>
+      <c r="E92" s="68"/>
+      <c r="F92" s="68"/>
+      <c r="G92" s="69"/>
       <c r="H92" s="12" t="s">
         <v>58</v>
       </c>
@@ -6783,11 +6789,11 @@
       <c r="B93" s="27">
         <v>72</v>
       </c>
-      <c r="C93" s="93"/>
-      <c r="D93" s="75"/>
-      <c r="E93" s="75"/>
-      <c r="F93" s="75"/>
-      <c r="G93" s="76"/>
+      <c r="C93" s="86"/>
+      <c r="D93" s="68"/>
+      <c r="E93" s="68"/>
+      <c r="F93" s="68"/>
+      <c r="G93" s="69"/>
       <c r="H93" s="12" t="s">
         <v>58</v>
       </c>
@@ -6796,11 +6802,11 @@
       <c r="B94" s="9">
         <v>73</v>
       </c>
-      <c r="C94" s="93"/>
-      <c r="D94" s="75"/>
-      <c r="E94" s="75"/>
-      <c r="F94" s="75"/>
-      <c r="G94" s="76"/>
+      <c r="C94" s="86"/>
+      <c r="D94" s="68"/>
+      <c r="E94" s="68"/>
+      <c r="F94" s="68"/>
+      <c r="G94" s="69"/>
       <c r="H94" s="12" t="s">
         <v>58</v>
       </c>
@@ -6809,11 +6815,11 @@
       <c r="B95" s="27">
         <v>74</v>
       </c>
-      <c r="C95" s="93"/>
-      <c r="D95" s="75"/>
-      <c r="E95" s="75"/>
-      <c r="F95" s="75"/>
-      <c r="G95" s="76"/>
+      <c r="C95" s="86"/>
+      <c r="D95" s="68"/>
+      <c r="E95" s="68"/>
+      <c r="F95" s="68"/>
+      <c r="G95" s="69"/>
       <c r="H95" s="12" t="s">
         <v>58</v>
       </c>
@@ -6822,11 +6828,11 @@
       <c r="B96" s="9">
         <v>75</v>
       </c>
-      <c r="C96" s="93"/>
-      <c r="D96" s="75"/>
-      <c r="E96" s="75"/>
-      <c r="F96" s="75"/>
-      <c r="G96" s="76"/>
+      <c r="C96" s="86"/>
+      <c r="D96" s="68"/>
+      <c r="E96" s="68"/>
+      <c r="F96" s="68"/>
+      <c r="G96" s="69"/>
       <c r="H96" s="12" t="s">
         <v>58</v>
       </c>
@@ -6835,11 +6841,11 @@
       <c r="B97" s="27">
         <v>76</v>
       </c>
-      <c r="C97" s="93"/>
-      <c r="D97" s="75"/>
-      <c r="E97" s="75"/>
-      <c r="F97" s="75"/>
-      <c r="G97" s="76"/>
+      <c r="C97" s="86"/>
+      <c r="D97" s="68"/>
+      <c r="E97" s="68"/>
+      <c r="F97" s="68"/>
+      <c r="G97" s="69"/>
       <c r="H97" s="12" t="s">
         <v>58</v>
       </c>
@@ -6848,11 +6854,11 @@
       <c r="B98" s="9">
         <v>77</v>
       </c>
-      <c r="C98" s="93"/>
-      <c r="D98" s="75"/>
-      <c r="E98" s="75"/>
-      <c r="F98" s="75"/>
-      <c r="G98" s="76"/>
+      <c r="C98" s="86"/>
+      <c r="D98" s="68"/>
+      <c r="E98" s="68"/>
+      <c r="F98" s="68"/>
+      <c r="G98" s="69"/>
       <c r="H98" s="12" t="s">
         <v>58</v>
       </c>
@@ -6861,11 +6867,11 @@
       <c r="B99" s="27">
         <v>78</v>
       </c>
-      <c r="C99" s="93"/>
-      <c r="D99" s="75"/>
-      <c r="E99" s="75"/>
-      <c r="F99" s="75"/>
-      <c r="G99" s="76"/>
+      <c r="C99" s="86"/>
+      <c r="D99" s="68"/>
+      <c r="E99" s="68"/>
+      <c r="F99" s="68"/>
+      <c r="G99" s="69"/>
       <c r="H99" s="12" t="s">
         <v>58</v>
       </c>
@@ -6874,11 +6880,11 @@
       <c r="B100" s="9">
         <v>79</v>
       </c>
-      <c r="C100" s="93"/>
-      <c r="D100" s="75"/>
-      <c r="E100" s="75"/>
-      <c r="F100" s="75"/>
-      <c r="G100" s="76"/>
+      <c r="C100" s="86"/>
+      <c r="D100" s="68"/>
+      <c r="E100" s="68"/>
+      <c r="F100" s="68"/>
+      <c r="G100" s="69"/>
       <c r="H100" s="12" t="s">
         <v>58</v>
       </c>
@@ -6887,11 +6893,11 @@
       <c r="B101" s="27">
         <v>80</v>
       </c>
-      <c r="C101" s="93"/>
-      <c r="D101" s="75"/>
-      <c r="E101" s="75"/>
-      <c r="F101" s="75"/>
-      <c r="G101" s="76"/>
+      <c r="C101" s="86"/>
+      <c r="D101" s="68"/>
+      <c r="E101" s="68"/>
+      <c r="F101" s="68"/>
+      <c r="G101" s="69"/>
       <c r="H101" s="12" t="s">
         <v>58</v>
       </c>
@@ -6900,11 +6906,11 @@
       <c r="B102" s="9">
         <v>81</v>
       </c>
-      <c r="C102" s="93"/>
-      <c r="D102" s="75"/>
-      <c r="E102" s="75"/>
-      <c r="F102" s="75"/>
-      <c r="G102" s="76"/>
+      <c r="C102" s="86"/>
+      <c r="D102" s="68"/>
+      <c r="E102" s="68"/>
+      <c r="F102" s="68"/>
+      <c r="G102" s="69"/>
       <c r="H102" s="12" t="s">
         <v>58</v>
       </c>
@@ -6913,11 +6919,11 @@
       <c r="B103" s="27">
         <v>82</v>
       </c>
-      <c r="C103" s="93"/>
-      <c r="D103" s="75"/>
-      <c r="E103" s="75"/>
-      <c r="F103" s="75"/>
-      <c r="G103" s="76"/>
+      <c r="C103" s="86"/>
+      <c r="D103" s="68"/>
+      <c r="E103" s="68"/>
+      <c r="F103" s="68"/>
+      <c r="G103" s="69"/>
       <c r="H103" s="12" t="s">
         <v>58</v>
       </c>
@@ -6926,11 +6932,11 @@
       <c r="B104" s="9">
         <v>83</v>
       </c>
-      <c r="C104" s="93"/>
-      <c r="D104" s="75"/>
-      <c r="E104" s="75"/>
-      <c r="F104" s="75"/>
-      <c r="G104" s="76"/>
+      <c r="C104" s="86"/>
+      <c r="D104" s="68"/>
+      <c r="E104" s="68"/>
+      <c r="F104" s="68"/>
+      <c r="G104" s="69"/>
       <c r="H104" s="12" t="s">
         <v>58</v>
       </c>
@@ -6939,11 +6945,11 @@
       <c r="B105" s="27">
         <v>84</v>
       </c>
-      <c r="C105" s="93"/>
-      <c r="D105" s="75"/>
-      <c r="E105" s="75"/>
-      <c r="F105" s="75"/>
-      <c r="G105" s="76"/>
+      <c r="C105" s="86"/>
+      <c r="D105" s="68"/>
+      <c r="E105" s="68"/>
+      <c r="F105" s="68"/>
+      <c r="G105" s="69"/>
       <c r="H105" s="12" t="s">
         <v>58</v>
       </c>
@@ -6952,11 +6958,11 @@
       <c r="B106" s="9">
         <v>85</v>
       </c>
-      <c r="C106" s="93"/>
-      <c r="D106" s="75"/>
-      <c r="E106" s="75"/>
-      <c r="F106" s="75"/>
-      <c r="G106" s="76"/>
+      <c r="C106" s="86"/>
+      <c r="D106" s="68"/>
+      <c r="E106" s="68"/>
+      <c r="F106" s="68"/>
+      <c r="G106" s="69"/>
       <c r="H106" s="12" t="s">
         <v>58</v>
       </c>
@@ -6965,11 +6971,11 @@
       <c r="B107" s="27">
         <v>86</v>
       </c>
-      <c r="C107" s="93"/>
-      <c r="D107" s="75"/>
-      <c r="E107" s="75"/>
-      <c r="F107" s="75"/>
-      <c r="G107" s="76"/>
+      <c r="C107" s="86"/>
+      <c r="D107" s="68"/>
+      <c r="E107" s="68"/>
+      <c r="F107" s="68"/>
+      <c r="G107" s="69"/>
       <c r="H107" s="12" t="s">
         <v>58</v>
       </c>
@@ -6978,11 +6984,11 @@
       <c r="B108" s="9">
         <v>87</v>
       </c>
-      <c r="C108" s="93"/>
-      <c r="D108" s="75"/>
-      <c r="E108" s="75"/>
-      <c r="F108" s="75"/>
-      <c r="G108" s="76"/>
+      <c r="C108" s="86"/>
+      <c r="D108" s="68"/>
+      <c r="E108" s="68"/>
+      <c r="F108" s="68"/>
+      <c r="G108" s="69"/>
       <c r="H108" s="12" t="s">
         <v>58</v>
       </c>
@@ -6991,11 +6997,11 @@
       <c r="B109" s="27">
         <v>88</v>
       </c>
-      <c r="C109" s="93"/>
-      <c r="D109" s="75"/>
-      <c r="E109" s="75"/>
-      <c r="F109" s="75"/>
-      <c r="G109" s="76"/>
+      <c r="C109" s="86"/>
+      <c r="D109" s="68"/>
+      <c r="E109" s="68"/>
+      <c r="F109" s="68"/>
+      <c r="G109" s="69"/>
       <c r="H109" s="12" t="s">
         <v>58</v>
       </c>
@@ -7004,11 +7010,11 @@
       <c r="B110" s="9">
         <v>89</v>
       </c>
-      <c r="C110" s="93"/>
-      <c r="D110" s="75"/>
-      <c r="E110" s="75"/>
-      <c r="F110" s="75"/>
-      <c r="G110" s="76"/>
+      <c r="C110" s="86"/>
+      <c r="D110" s="68"/>
+      <c r="E110" s="68"/>
+      <c r="F110" s="68"/>
+      <c r="G110" s="69"/>
       <c r="H110" s="12" t="s">
         <v>58</v>
       </c>
@@ -7017,11 +7023,11 @@
       <c r="B111" s="27">
         <v>90</v>
       </c>
-      <c r="C111" s="93"/>
-      <c r="D111" s="75"/>
-      <c r="E111" s="75"/>
-      <c r="F111" s="75"/>
-      <c r="G111" s="76"/>
+      <c r="C111" s="86"/>
+      <c r="D111" s="68"/>
+      <c r="E111" s="68"/>
+      <c r="F111" s="68"/>
+      <c r="G111" s="69"/>
       <c r="H111" s="12" t="s">
         <v>58</v>
       </c>
@@ -7030,11 +7036,11 @@
       <c r="B112" s="9">
         <v>91</v>
       </c>
-      <c r="C112" s="93"/>
-      <c r="D112" s="75"/>
-      <c r="E112" s="75"/>
-      <c r="F112" s="75"/>
-      <c r="G112" s="76"/>
+      <c r="C112" s="86"/>
+      <c r="D112" s="68"/>
+      <c r="E112" s="68"/>
+      <c r="F112" s="68"/>
+      <c r="G112" s="69"/>
       <c r="H112" s="12" t="s">
         <v>58</v>
       </c>
@@ -7043,11 +7049,11 @@
       <c r="B113" s="27">
         <v>92</v>
       </c>
-      <c r="C113" s="93"/>
-      <c r="D113" s="75"/>
-      <c r="E113" s="75"/>
-      <c r="F113" s="75"/>
-      <c r="G113" s="76"/>
+      <c r="C113" s="86"/>
+      <c r="D113" s="68"/>
+      <c r="E113" s="68"/>
+      <c r="F113" s="68"/>
+      <c r="G113" s="69"/>
       <c r="H113" s="12" t="s">
         <v>58</v>
       </c>
@@ -7056,11 +7062,11 @@
       <c r="B114" s="9">
         <v>93</v>
       </c>
-      <c r="C114" s="93"/>
-      <c r="D114" s="75"/>
-      <c r="E114" s="75"/>
-      <c r="F114" s="75"/>
-      <c r="G114" s="76"/>
+      <c r="C114" s="86"/>
+      <c r="D114" s="68"/>
+      <c r="E114" s="68"/>
+      <c r="F114" s="68"/>
+      <c r="G114" s="69"/>
       <c r="H114" s="12" t="s">
         <v>58</v>
       </c>
@@ -7069,11 +7075,11 @@
       <c r="B115" s="27">
         <v>94</v>
       </c>
-      <c r="C115" s="93"/>
-      <c r="D115" s="75"/>
-      <c r="E115" s="75"/>
-      <c r="F115" s="75"/>
-      <c r="G115" s="76"/>
+      <c r="C115" s="86"/>
+      <c r="D115" s="68"/>
+      <c r="E115" s="68"/>
+      <c r="F115" s="68"/>
+      <c r="G115" s="69"/>
       <c r="H115" s="12" t="s">
         <v>58</v>
       </c>
@@ -7082,11 +7088,11 @@
       <c r="B116" s="9">
         <v>95</v>
       </c>
-      <c r="C116" s="93"/>
-      <c r="D116" s="75"/>
-      <c r="E116" s="75"/>
-      <c r="F116" s="75"/>
-      <c r="G116" s="76"/>
+      <c r="C116" s="86"/>
+      <c r="D116" s="68"/>
+      <c r="E116" s="68"/>
+      <c r="F116" s="68"/>
+      <c r="G116" s="69"/>
       <c r="H116" s="12" t="s">
         <v>58</v>
       </c>
@@ -7095,11 +7101,11 @@
       <c r="B117" s="27">
         <v>96</v>
       </c>
-      <c r="C117" s="93"/>
-      <c r="D117" s="75"/>
-      <c r="E117" s="75"/>
-      <c r="F117" s="75"/>
-      <c r="G117" s="76"/>
+      <c r="C117" s="86"/>
+      <c r="D117" s="68"/>
+      <c r="E117" s="68"/>
+      <c r="F117" s="68"/>
+      <c r="G117" s="69"/>
       <c r="H117" s="12" t="s">
         <v>58</v>
       </c>
@@ -7108,11 +7114,11 @@
       <c r="B118" s="9">
         <v>97</v>
       </c>
-      <c r="C118" s="93"/>
-      <c r="D118" s="75"/>
-      <c r="E118" s="75"/>
-      <c r="F118" s="75"/>
-      <c r="G118" s="76"/>
+      <c r="C118" s="86"/>
+      <c r="D118" s="68"/>
+      <c r="E118" s="68"/>
+      <c r="F118" s="68"/>
+      <c r="G118" s="69"/>
       <c r="H118" s="12" t="s">
         <v>58</v>
       </c>
@@ -7121,11 +7127,11 @@
       <c r="B119" s="27">
         <v>98</v>
       </c>
-      <c r="C119" s="93"/>
-      <c r="D119" s="75"/>
-      <c r="E119" s="75"/>
-      <c r="F119" s="75"/>
-      <c r="G119" s="76"/>
+      <c r="C119" s="86"/>
+      <c r="D119" s="68"/>
+      <c r="E119" s="68"/>
+      <c r="F119" s="68"/>
+      <c r="G119" s="69"/>
       <c r="H119" s="12" t="s">
         <v>58</v>
       </c>
@@ -7134,11 +7140,11 @@
       <c r="B120" s="9">
         <v>99</v>
       </c>
-      <c r="C120" s="93"/>
-      <c r="D120" s="75"/>
-      <c r="E120" s="75"/>
-      <c r="F120" s="75"/>
-      <c r="G120" s="76"/>
+      <c r="C120" s="86"/>
+      <c r="D120" s="68"/>
+      <c r="E120" s="68"/>
+      <c r="F120" s="68"/>
+      <c r="G120" s="69"/>
       <c r="H120" s="12" t="s">
         <v>58</v>
       </c>
@@ -7147,11 +7153,11 @@
       <c r="B121" s="27">
         <v>100</v>
       </c>
-      <c r="C121" s="93"/>
-      <c r="D121" s="75"/>
-      <c r="E121" s="75"/>
-      <c r="F121" s="75"/>
-      <c r="G121" s="76"/>
+      <c r="C121" s="86"/>
+      <c r="D121" s="68"/>
+      <c r="E121" s="68"/>
+      <c r="F121" s="68"/>
+      <c r="G121" s="69"/>
       <c r="H121" s="12" t="s">
         <v>58</v>
       </c>
@@ -8830,53 +8836,51 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="116">
-    <mergeCell ref="C97:G97"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="C99:G99"/>
-    <mergeCell ref="C100:G100"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="C88:G88"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="C96:G96"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="C80:G80"/>
-    <mergeCell ref="C81:G81"/>
-    <mergeCell ref="C82:G82"/>
-    <mergeCell ref="C83:G83"/>
-    <mergeCell ref="C84:G84"/>
-    <mergeCell ref="C85:G85"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="C120:G120"/>
-    <mergeCell ref="C121:G121"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="C113:G113"/>
-    <mergeCell ref="C114:G114"/>
-    <mergeCell ref="C115:G115"/>
-    <mergeCell ref="C116:G116"/>
-    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:G50"/>
     <mergeCell ref="C51:G51"/>
     <mergeCell ref="C52:G52"/>
     <mergeCell ref="C53:G53"/>
@@ -8901,51 +8905,53 @@
     <mergeCell ref="C67:G67"/>
     <mergeCell ref="C68:G68"/>
     <mergeCell ref="C69:G69"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="C120:G120"/>
+    <mergeCell ref="C121:G121"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="C113:G113"/>
+    <mergeCell ref="C114:G114"/>
+    <mergeCell ref="C115:G115"/>
+    <mergeCell ref="C116:G116"/>
+    <mergeCell ref="C117:G117"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="C80:G80"/>
+    <mergeCell ref="C81:G81"/>
+    <mergeCell ref="C82:G82"/>
+    <mergeCell ref="C83:G83"/>
+    <mergeCell ref="C84:G84"/>
+    <mergeCell ref="C85:G85"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="C99:G99"/>
+    <mergeCell ref="C100:G100"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="C88:G88"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="C96:G96"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H22:H121" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8994,85 +9000,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="B1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="81"/>
       <c r="K1" s="2">
         <f>Requisitos!C11</f>
         <v>44796</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="83"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>44797</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>44798</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="75"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>44799</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>44800</v>
@@ -9086,18 +9092,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="74" t="str">
+      <c r="B7" s="76" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Sistema Atelier Picinin</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>44802</v>
@@ -9111,16 +9117,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
       <c r="J9" s="57" t="s">
         <v>74</v>
       </c>
@@ -10202,26 +10208,26 @@
       <c r="J62" s="5"/>
     </row>
     <row r="63" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="95" t="s">
+      <c r="B63" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="C63" s="75"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="75"/>
-      <c r="I63" s="76"/>
+      <c r="C63" s="68"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="68"/>
+      <c r="G63" s="68"/>
+      <c r="H63" s="68"/>
+      <c r="I63" s="69"/>
     </row>
     <row r="64" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="96" t="s">
+      <c r="B64" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="76"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="68"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="69"/>
       <c r="H64" s="7" t="s">
         <v>93</v>
       </c>
@@ -10230,15 +10236,15 @@
       </c>
     </row>
     <row r="65" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="94" t="str">
+      <c r="B65" s="95" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Lucas Picinin Campos Lutti</v>
       </c>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="76"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="69"/>
       <c r="H65" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -10249,15 +10255,15 @@
       </c>
     </row>
     <row r="66" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="94" t="str">
+      <c r="B66" s="95" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v xml:space="preserve">Gabriel Lima </v>
       </c>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="76"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="69"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>146</v>
@@ -10268,15 +10274,15 @@
       </c>
     </row>
     <row r="67" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="94" t="str">
+      <c r="B67" s="95" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v xml:space="preserve">Gabriel de Souza </v>
       </c>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="76"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="69"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>216</v>
@@ -10287,15 +10293,15 @@
       </c>
     </row>
     <row r="68" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="94" t="str">
+      <c r="B68" s="95" t="str">
         <f>'Dados do Projeto'!B13</f>
         <v xml:space="preserve">Nikolas Louret </v>
       </c>
-      <c r="C68" s="75"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="76"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="69"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -10306,15 +10312,15 @@
       </c>
     </row>
     <row r="69" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="94">
+      <c r="B69" s="95">
         <f>'Dados do Projeto'!B14</f>
         <v>0</v>
       </c>
-      <c r="C69" s="75"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="76"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="69"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -11451,85 +11457,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="B1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="81"/>
       <c r="K1" s="2">
         <f>Requisitos!C12</f>
         <v>44810</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="83"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>44811</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>44812</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="75"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>44813</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>44814</v>
@@ -11543,18 +11549,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B7" s="74" t="str">
+      <c r="B7" s="76" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Sistema Atelier Picinin</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>44816</v>
@@ -11568,16 +11574,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="96" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
       <c r="J9" s="57" t="s">
         <v>74</v>
       </c>
@@ -12769,26 +12775,26 @@
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="95" t="s">
+      <c r="B72" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="C72" s="75"/>
-      <c r="D72" s="75"/>
-      <c r="E72" s="75"/>
-      <c r="F72" s="75"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
-      <c r="I72" s="76"/>
+      <c r="C72" s="68"/>
+      <c r="D72" s="68"/>
+      <c r="E72" s="68"/>
+      <c r="F72" s="68"/>
+      <c r="G72" s="68"/>
+      <c r="H72" s="68"/>
+      <c r="I72" s="69"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="96" t="s">
+      <c r="B73" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="C73" s="75"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
-      <c r="G73" s="76"/>
+      <c r="C73" s="68"/>
+      <c r="D73" s="68"/>
+      <c r="E73" s="68"/>
+      <c r="F73" s="68"/>
+      <c r="G73" s="69"/>
       <c r="H73" s="7" t="s">
         <v>93</v>
       </c>
@@ -12797,15 +12803,15 @@
       </c>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="94" t="str">
+      <c r="B74" s="95" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Lucas Picinin Campos Lutti</v>
       </c>
-      <c r="C74" s="75"/>
-      <c r="D74" s="75"/>
-      <c r="E74" s="75"/>
-      <c r="F74" s="75"/>
-      <c r="G74" s="76"/>
+      <c r="C74" s="68"/>
+      <c r="D74" s="68"/>
+      <c r="E74" s="68"/>
+      <c r="F74" s="68"/>
+      <c r="G74" s="69"/>
       <c r="H74" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -12816,15 +12822,15 @@
       </c>
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="94" t="str">
+      <c r="B75" s="95" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v xml:space="preserve">Gabriel Lima </v>
       </c>
-      <c r="C75" s="75"/>
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
-      <c r="F75" s="75"/>
-      <c r="G75" s="76"/>
+      <c r="C75" s="68"/>
+      <c r="D75" s="68"/>
+      <c r="E75" s="68"/>
+      <c r="F75" s="68"/>
+      <c r="G75" s="69"/>
       <c r="H75" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -12835,15 +12841,15 @@
       </c>
     </row>
     <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="94" t="str">
+      <c r="B76" s="95" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v xml:space="preserve">Gabriel de Souza </v>
       </c>
-      <c r="C76" s="75"/>
-      <c r="D76" s="75"/>
-      <c r="E76" s="75"/>
-      <c r="F76" s="75"/>
-      <c r="G76" s="76"/>
+      <c r="C76" s="68"/>
+      <c r="D76" s="68"/>
+      <c r="E76" s="68"/>
+      <c r="F76" s="68"/>
+      <c r="G76" s="69"/>
       <c r="H76" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -12854,15 +12860,15 @@
       </c>
     </row>
     <row r="77" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="94" t="str">
+      <c r="B77" s="95" t="str">
         <f>'Dados do Projeto'!B13</f>
         <v xml:space="preserve">Nikolas Louret </v>
       </c>
-      <c r="C77" s="75"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
-      <c r="F77" s="75"/>
-      <c r="G77" s="76"/>
+      <c r="C77" s="68"/>
+      <c r="D77" s="68"/>
+      <c r="E77" s="68"/>
+      <c r="F77" s="68"/>
+      <c r="G77" s="69"/>
       <c r="H77" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -12873,15 +12879,15 @@
       </c>
     </row>
     <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="94">
+      <c r="B78" s="95">
         <f>'Dados do Projeto'!B14</f>
         <v>0</v>
       </c>
-      <c r="C78" s="75"/>
-      <c r="D78" s="75"/>
-      <c r="E78" s="75"/>
-      <c r="F78" s="75"/>
-      <c r="G78" s="76"/>
+      <c r="C78" s="68"/>
+      <c r="D78" s="68"/>
+      <c r="E78" s="68"/>
+      <c r="F78" s="68"/>
+      <c r="G78" s="69"/>
       <c r="H78" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -14107,85 +14113,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="B1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="81"/>
       <c r="K1" s="2">
         <f>Requisitos!C13</f>
         <v>44824</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="83"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>44825</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>44826</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="75"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>44827</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>44828</v>
@@ -14198,18 +14204,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="74" t="str">
+      <c r="B7" s="76" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Sistema Atelier Picinin</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>44830</v>
@@ -14222,16 +14228,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
       <c r="J9" s="58" t="s">
         <v>74</v>
       </c>
@@ -15249,26 +15255,26 @@
       </c>
     </row>
     <row r="63" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="95" t="s">
+      <c r="B63" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="C63" s="75"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="75"/>
-      <c r="I63" s="76"/>
+      <c r="C63" s="68"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="68"/>
+      <c r="G63" s="68"/>
+      <c r="H63" s="68"/>
+      <c r="I63" s="69"/>
     </row>
     <row r="64" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="96" t="s">
+      <c r="B64" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="76"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="68"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="69"/>
       <c r="H64" s="7" t="s">
         <v>93</v>
       </c>
@@ -15277,15 +15283,15 @@
       </c>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="94" t="str">
+      <c r="B65" s="95" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Lucas Picinin Campos Lutti</v>
       </c>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="76"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="69"/>
       <c r="H65" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -15296,15 +15302,15 @@
       </c>
     </row>
     <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="94" t="str">
+      <c r="B66" s="95" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v xml:space="preserve">Gabriel Lima </v>
       </c>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="76"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="69"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -15315,15 +15321,15 @@
       </c>
     </row>
     <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="94" t="str">
+      <c r="B67" s="95" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v xml:space="preserve">Gabriel de Souza </v>
       </c>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="76"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="69"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -15334,15 +15340,15 @@
       </c>
     </row>
     <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="94" t="str">
+      <c r="B68" s="95" t="str">
         <f>'Dados do Projeto'!B13</f>
         <v xml:space="preserve">Nikolas Louret </v>
       </c>
-      <c r="C68" s="75"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="76"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="69"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -15353,15 +15359,15 @@
       </c>
     </row>
     <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="94">
+      <c r="B69" s="95">
         <f>'Dados do Projeto'!B14</f>
         <v>0</v>
       </c>
-      <c r="C69" s="75"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="76"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="69"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -16705,9 +16711,9 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16726,85 +16732,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="B1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="81"/>
       <c r="K1" s="2">
         <f>Requisitos!C14</f>
         <v>44838</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="83"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K21" si="0">K1+1</f>
         <v>44839</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>44840</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="75"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>44841</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>44842</v>
@@ -16817,18 +16823,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="74" t="str">
+      <c r="B7" s="76" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Sistema Atelier Picinin</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>44844</v>
@@ -16841,16 +16847,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
       <c r="J9" s="58" t="s">
         <v>74</v>
       </c>
@@ -17013,7 +17019,7 @@
       <c r="I14" s="13">
         <v>10</v>
       </c>
-      <c r="J14" s="97"/>
+      <c r="J14" s="64"/>
       <c r="K14" s="2">
         <f t="shared" si="0"/>
         <v>44851</v>
@@ -17896,26 +17902,26 @@
       </c>
     </row>
     <row r="63" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="95" t="s">
+      <c r="B63" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="C63" s="75"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="75"/>
-      <c r="I63" s="76"/>
+      <c r="C63" s="68"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="68"/>
+      <c r="G63" s="68"/>
+      <c r="H63" s="68"/>
+      <c r="I63" s="69"/>
     </row>
     <row r="64" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="96" t="s">
+      <c r="B64" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="76"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="68"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="69"/>
       <c r="H64" s="7" t="s">
         <v>93</v>
       </c>
@@ -17924,15 +17930,15 @@
       </c>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="94" t="str">
+      <c r="B65" s="95" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Lucas Picinin Campos Lutti</v>
       </c>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="76"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="69"/>
       <c r="H65" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -17943,15 +17949,15 @@
       </c>
     </row>
     <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="94" t="str">
+      <c r="B66" s="95" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v xml:space="preserve">Gabriel Lima </v>
       </c>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="76"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="69"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -17962,15 +17968,15 @@
       </c>
     </row>
     <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="94" t="str">
+      <c r="B67" s="95" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v xml:space="preserve">Gabriel de Souza </v>
       </c>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="76"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="69"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -17981,15 +17987,15 @@
       </c>
     </row>
     <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="94" t="str">
+      <c r="B68" s="95" t="str">
         <f>'Dados do Projeto'!B13</f>
         <v xml:space="preserve">Nikolas Louret </v>
       </c>
-      <c r="C68" s="75"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="76"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="69"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -18000,15 +18006,15 @@
       </c>
     </row>
     <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="94">
+      <c r="B69" s="95">
         <f>'Dados do Projeto'!B14</f>
         <v>0</v>
       </c>
-      <c r="C69" s="75"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="76"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="69"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -19212,9 +19218,9 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -19234,85 +19240,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="B1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="81"/>
       <c r="K1" s="2">
         <f>Requisitos!C15</f>
         <v>44859</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="83"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>44860</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>44861</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="75"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>44862</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>44863</v>
@@ -19325,18 +19331,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="74" t="str">
+      <c r="B7" s="76" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Sistema Atelier Picinin</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>44865</v>
@@ -19349,16 +19355,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
       <c r="J9" s="58" t="s">
         <v>74</v>
       </c>
@@ -19636,12 +19642,20 @@
         <v>9</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H19" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="13">
         <v>0</v>
@@ -19654,12 +19668,20 @@
         <v>10</v>
       </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="D20" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="H20" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="13">
         <v>0</v>
@@ -20361,7 +20383,7 @@
       </c>
       <c r="H61" s="32">
         <f t="shared" ref="H61:I61" si="1">SUM(H11:H60)</f>
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I61" s="32">
         <f t="shared" si="1"/>
@@ -20373,7 +20395,7 @@
       <c r="C62" s="30"/>
       <c r="D62" s="30">
         <f>COUNTIFS(D11:D60, "&lt;&gt;"&amp;"")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E62" s="30"/>
       <c r="F62" s="30"/>
@@ -20383,26 +20405,26 @@
       </c>
     </row>
     <row r="63" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="95" t="s">
+      <c r="B63" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="C63" s="75"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="75"/>
-      <c r="I63" s="76"/>
+      <c r="C63" s="68"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="68"/>
+      <c r="G63" s="68"/>
+      <c r="H63" s="68"/>
+      <c r="I63" s="69"/>
     </row>
     <row r="64" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="96" t="s">
+      <c r="B64" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="76"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="68"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="69"/>
       <c r="H64" s="7" t="s">
         <v>93</v>
       </c>
@@ -20411,15 +20433,15 @@
       </c>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="94" t="str">
+      <c r="B65" s="95" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Lucas Picinin Campos Lutti</v>
       </c>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="76"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="69"/>
       <c r="H65" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -20430,15 +20452,15 @@
       </c>
     </row>
     <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="94" t="str">
+      <c r="B66" s="95" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v xml:space="preserve">Gabriel Lima </v>
       </c>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="76"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="69"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -20449,15 +20471,15 @@
       </c>
     </row>
     <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="94" t="str">
+      <c r="B67" s="95" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v xml:space="preserve">Gabriel de Souza </v>
       </c>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="76"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="69"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -20468,15 +20490,15 @@
       </c>
     </row>
     <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="94" t="str">
+      <c r="B68" s="95" t="str">
         <f>'Dados do Projeto'!B13</f>
         <v xml:space="preserve">Nikolas Louret </v>
       </c>
-      <c r="C68" s="75"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="76"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="69"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -20487,15 +20509,15 @@
       </c>
     </row>
     <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="94">
+      <c r="B69" s="95">
         <f>'Dados do Projeto'!B14</f>
         <v>0</v>
       </c>
-      <c r="C69" s="75"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="76"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="69"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>
@@ -21458,12 +21480,6 @@
   </sheetData>
   <autoFilter ref="B10:J60" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <mergeCells count="14">
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
     <mergeCell ref="B68:G68"/>
     <mergeCell ref="B69:G69"/>
     <mergeCell ref="B9:I9"/>
@@ -21472,6 +21488,12 @@
     <mergeCell ref="B65:G65"/>
     <mergeCell ref="B66:G66"/>
     <mergeCell ref="B67:G67"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="F13 F17">
     <cfRule type="containsBlanks" dxfId="75" priority="1">
@@ -21680,7 +21702,7 @@
           <x14:formula1>
             <xm:f>'Dados do Projeto'!$M$100:$M$103</xm:f>
           </x14:formula1>
-          <xm:sqref>G11:G18</xm:sqref>
+          <xm:sqref>G11:G20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -21720,85 +21742,85 @@
   <sheetData>
     <row r="1" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="B1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="81"/>
       <c r="K1" s="2">
         <f>Requisitos!C16</f>
         <v>44873</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="83"/>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K14" si="0">K1+1</f>
         <v>44874</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="83"/>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
         <v>44875</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="75"/>
       <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>44876</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
         <v>44877</v>
@@ -21811,18 +21833,18 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="74" t="str">
+      <c r="B7" s="76" t="str">
         <f>'Dados do Projeto'!B7</f>
         <v>Sistema Atelier Picinin</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="76"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
       <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>44879</v>
@@ -21835,16 +21857,16 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="96" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="76"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
       <c r="J9" s="58" t="s">
         <v>74</v>
       </c>
@@ -22805,26 +22827,26 @@
       </c>
     </row>
     <row r="63" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="95" t="s">
+      <c r="B63" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="C63" s="75"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="75"/>
-      <c r="I63" s="76"/>
+      <c r="C63" s="68"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="68"/>
+      <c r="G63" s="68"/>
+      <c r="H63" s="68"/>
+      <c r="I63" s="69"/>
     </row>
     <row r="64" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="96" t="s">
+      <c r="B64" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="76"/>
+      <c r="C64" s="68"/>
+      <c r="D64" s="68"/>
+      <c r="E64" s="68"/>
+      <c r="F64" s="68"/>
+      <c r="G64" s="69"/>
       <c r="H64" s="7" t="s">
         <v>93</v>
       </c>
@@ -22833,15 +22855,15 @@
       </c>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="94" t="str">
+      <c r="B65" s="95" t="str">
         <f>'Dados do Projeto'!B10</f>
         <v>Lucas Picinin Campos Lutti</v>
       </c>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="76"/>
+      <c r="C65" s="68"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="69"/>
       <c r="H65" s="33">
         <f>SUMIF($F$11:$F$60,'Dados do Projeto'!$B10,H$11:H$60)</f>
         <v>0</v>
@@ -22852,15 +22874,15 @@
       </c>
     </row>
     <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="94" t="str">
+      <c r="B66" s="95" t="str">
         <f>'Dados do Projeto'!B11</f>
         <v xml:space="preserve">Gabriel Lima </v>
       </c>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="76"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="68"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
+      <c r="G66" s="69"/>
       <c r="H66" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B11,H$11:H$60)</f>
         <v>0</v>
@@ -22871,15 +22893,15 @@
       </c>
     </row>
     <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="94" t="str">
+      <c r="B67" s="95" t="str">
         <f>'Dados do Projeto'!B12</f>
         <v xml:space="preserve">Gabriel de Souza </v>
       </c>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="76"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
+      <c r="G67" s="69"/>
       <c r="H67" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B12,H$11:H$60)</f>
         <v>0</v>
@@ -22890,15 +22912,15 @@
       </c>
     </row>
     <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="94" t="str">
+      <c r="B68" s="95" t="str">
         <f>'Dados do Projeto'!B13</f>
         <v xml:space="preserve">Nikolas Louret </v>
       </c>
-      <c r="C68" s="75"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="76"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="68"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="69"/>
       <c r="H68" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B13,H$11:H$60)</f>
         <v>0</v>
@@ -22909,15 +22931,15 @@
       </c>
     </row>
     <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="94">
+      <c r="B69" s="95">
         <f>'Dados do Projeto'!B14</f>
         <v>0</v>
       </c>
-      <c r="C69" s="75"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="76"/>
+      <c r="C69" s="68"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="68"/>
+      <c r="G69" s="69"/>
       <c r="H69" s="33">
         <f>SUMIF(F$11:F$60,'Dados do Projeto'!B14,H$11:H$60)</f>
         <v>0</v>

</xml_diff>